<commit_message>
16 View Videos Completed
</commit_message>
<xml_diff>
--- a/1_Info/Embeded Video Links.xlsx
+++ b/1_Info/Embeded Video Links.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="38460" yWindow="1160" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Experiment</t>
   </si>
@@ -41,9 +41,6 @@
     <t>&lt;iframe src="https://player.vimeo.com/video/</t>
   </si>
   <si>
-    <t>" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
     <t>https://vimeo.com/175554702/20f76fe235</t>
   </si>
   <si>
@@ -66,6 +63,36 @@
   </si>
   <si>
     <t>https://vimeo.com/175554716/527b3495f8</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/176226121/d76c0f4be8</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/176225772/6441d88ef9</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175554709/b03e806831</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175554710/b1d449bed5</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175554708/4647d2b2db</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175554706/fe8a1a8ef2</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175554705/400e226eb3</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175849908/00ec6c6867</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/175850249/cda867f897</t>
+  </si>
+  <si>
+    <t>" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
@@ -383,7 +410,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,20 +434,20 @@
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B7" si="0">CONCATENATE(C2,E2,D2)</f>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554702" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554702" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E7" si="1">LEFT(RIGHT(F2,LEN(F2)-18),LEN(RIGHT(F2,LEN(F2)-18))-11)</f>
         <v>175554702</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -429,96 +456,108 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554704" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554704" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
         <v>175554704</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="e">
+      <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554706" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="e">
+        <v>21</v>
+      </c>
+      <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>175554706</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="e">
+      <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554705" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="e">
+        <v>21</v>
+      </c>
+      <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>175554705</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="e">
+      <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175849908" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="e">
+        <v>21</v>
+      </c>
+      <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>175849908</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="e">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175850249" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="e">
+        <v>21</v>
+      </c>
+      <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>175850249</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -527,13 +566,13 @@
       </c>
       <c r="B8" t="str">
         <f>CONCATENATE(C8,E8,D8)</f>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554707" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554707" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E8" t="str">
         <f>LEFT(RIGHT(F8,LEN(F8)-18),LEN(RIGHT(F8,LEN(F8)-18))-11)</f>
@@ -547,57 +586,66 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="e">
+      <c r="B9" t="str">
         <f t="shared" ref="B9:B19" si="2">CONCATENATE(C9,E9,D9)</f>
-        <v>#VALUE!</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554709" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" t="e">
+        <v>21</v>
+      </c>
+      <c r="E9" t="str">
         <f t="shared" ref="E9:E19" si="3">LEFT(RIGHT(F9,LEN(F9)-18),LEN(RIGHT(F9,LEN(F9)-18))-11)</f>
-        <v>#VALUE!</v>
+        <v>175554709</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="B10" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554708" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" t="e">
+        <v>21</v>
+      </c>
+      <c r="E10" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>175554708</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="B11" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554710" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="e">
+        <v>21</v>
+      </c>
+      <c r="E11" t="str">
         <f>LEFT(RIGHT(F11,LEN(F11)-18),LEN(RIGHT(F11,LEN(F11)-18))-11)</f>
-        <v>#VALUE!</v>
+        <v>175554710</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -606,20 +654,20 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554711" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554711" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E12" t="str">
         <f>LEFT(RIGHT(F12,LEN(F12)-18),LEN(RIGHT(F12,LEN(F12)-18))-11)</f>
         <v>175554711</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -628,20 +676,20 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554712" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554712" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
         <v>175554712</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -650,20 +698,20 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554713" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554713" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
         <v>175554713</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -672,20 +720,20 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554714" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554714" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
         <v>175554714</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -694,20 +742,20 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554715" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554715" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
         <v>175554715</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -716,58 +764,64 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;iframe src="https://player.vimeo.com/video/175554716" width=640" height="360" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
+        <v>&lt;iframe src="https://player.vimeo.com/video/175554716" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="3"/>
         <v>175554716</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;iframe src="https://player.vimeo.com/video/176225772" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="e">
+        <v>21</v>
+      </c>
+      <c r="E18" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>176225772</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;iframe src="https://player.vimeo.com/video/176226121" width=1280" height="720" frameborder="0" webkitallowfullscreen mozallowfullscreen allowfullscreen&gt;&lt;/iframe&gt;</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" t="e">
+        <v>21</v>
+      </c>
+      <c r="E19" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>176226121</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>